<commit_message>
Worked on new CPL files for 12-12 arenas with vreg.
</commit_message>
<xml_diff>
--- a/development/arena_12-12_w_vreg/ni/ni_arena_12-12_v0p1/production/version_0p1_r1/bom_cpl_wo_global_parts/BOM_JLCPCB_ni_arena_12-12_v0p1_r1.xlsx
+++ b/development/arena_12-12_w_vreg/ni/ni_arena_12-12_v0p1/production/version_0p1_r1/bom_cpl_wo_global_parts/BOM_JLCPCB_ni_arena_12-12_v0p1_r1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -92,12 +92,15 @@
     <t xml:space="preserve">C1591</t>
   </si>
   <si>
-    <t xml:space="preserve">10uF Ceramic Capacitor</t>
+    <t xml:space="preserve">10uF Ceramic Capacitor, 25V</t>
   </si>
   <si>
     <t xml:space="preserve">C11, C14, C17, C20, C23, C26, C29, C32, C35, C38, C41, C44, C47, C48</t>
   </si>
   <si>
+    <t xml:space="preserve">C96446</t>
+  </si>
+  <si>
     <t xml:space="preserve">100nF Ceramic Capacitor</t>
   </si>
   <si>
@@ -110,12 +113,18 @@
     <t xml:space="preserve">C13, C16, C19, C22, C25, C28, C31, C34, C37, C40, C43, C46</t>
   </si>
   <si>
+    <t xml:space="preserve">C2762594</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.3uH Inductor</t>
   </si>
   <si>
     <t xml:space="preserve">L1, L2, L3, L4, L5, L6, L7, L8, L9, L10, L11, L12</t>
   </si>
   <si>
+    <t xml:space="preserve">SMD,7.2x6.6mm</t>
+  </si>
+  <si>
     <t xml:space="preserve">C5189747</t>
   </si>
   <si>
@@ -140,16 +149,22 @@
     <t xml:space="preserve">C4328</t>
   </si>
   <si>
-    <t xml:space="preserve">56.2k Resistor</t>
+    <t xml:space="preserve">56.2k Resistor, 0.1%</t>
   </si>
   <si>
     <t xml:space="preserve">R3, R5, R7, R9, R11, R13, R15, R17, R19, R21, R23, R25</t>
   </si>
   <si>
-    <t xml:space="preserve">10k Resistor</t>
+    <t xml:space="preserve">C705784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k Resistor, 0.1%</t>
   </si>
   <si>
     <t xml:space="preserve">R4, R6, R8, R10, R12, R14, R16, R18, R20, R22, R24, R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C95204</t>
   </si>
   <si>
     <t xml:space="preserve">MOSFET N-channel</t>
@@ -458,7 +473,7 @@
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="85.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="8.89"/>
@@ -510,47 +525,59 @@
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="1" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E4" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>12</v>
@@ -558,16 +585,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>1</v>
@@ -575,16 +602,16 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>1</v>
@@ -592,44 +619,50 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E9" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="11" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E11" s="8" t="n">
         <v>1</v>
@@ -638,16 +671,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>5</v>
@@ -655,16 +688,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>12</v>
@@ -672,16 +705,16 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>1</v>

</xml_diff>